<commit_message>
Add softube dynamics. Rename files
</commit_message>
<xml_diff>
--- a/Zones/IconPlatNano_KB_1.0/Mapping.xlsx
+++ b/Zones/IconPlatNano_KB_1.0/Mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/568db26a05cb3412/Documents/git/ReaperCSINano/Zones/IconPlatNano_KB_1.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="8_{2C3CFBA9-8DED-4A44-A1DE-1044D74B9366}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D05808A0-8BF2-42DB-8A05-3A2FBDDA1EF1}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="8_{2C3CFBA9-8DED-4A44-A1DE-1044D74B9366}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{FB6B8FED-0697-4784-87D1-8ABBABCF1527}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="2205" windowWidth="19710" windowHeight="14145" xr2:uid="{D7A7375A-96C4-43BD-907F-7B9A83A15B3C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{D7A7375A-96C4-43BD-907F-7B9A83A15B3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="88">
   <si>
     <t>Rotary</t>
   </si>
@@ -289,6 +289,15 @@
   </si>
   <si>
     <t>Rend Queue</t>
+  </si>
+  <si>
+    <t>FX Zone</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Lock Item</t>
   </si>
 </sst>
 </file>
@@ -847,7 +856,7 @@
   <dimension ref="A2:N48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="N40" sqref="N40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -864,7 +873,7 @@
     <col min="10" max="10" width="9.140625" style="15"/>
     <col min="11" max="11" width="14.140625" style="15" customWidth="1"/>
     <col min="12" max="13" width="9.140625" style="15"/>
-    <col min="14" max="14" width="11" style="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" style="15" customWidth="1"/>
     <col min="15" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
@@ -1405,7 +1414,9 @@
       <c r="H21" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="I21" s="4"/>
+      <c r="I21" s="4" t="s">
+        <v>85</v>
+      </c>
       <c r="J21" s="26" t="s">
         <v>6</v>
       </c>
@@ -1436,7 +1447,9 @@
       <c r="H22" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="I22" s="6"/>
+      <c r="I22" s="6" t="s">
+        <v>86</v>
+      </c>
       <c r="J22" s="27" t="s">
         <v>7</v>
       </c>
@@ -1943,7 +1956,9 @@
       <c r="M40" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="N40" s="4"/>
+      <c r="N40" s="5" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>

</xml_diff>